<commit_message>
Added the pdf version of the excel
</commit_message>
<xml_diff>
--- a/Questao_01/Questao_01_Newton/Questao_01_1o_intervalo_newton.xlsx
+++ b/Questao_01/Questao_01_Newton/Questao_01_1o_intervalo_newton.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalvani\PycharmProjects\trabalho_calcl_numerico\Questao_01\Questao_01_Newton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalvani\Desktop\1o_trabalho_calculo_numerico\Primeiro_trabalho_calculo_numerico\Questao_01\Questao_01_Newton\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,14 +96,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="x_barra" dataDxfId="3"/>
-    <tableColumn id="2" name="f(x_barra)" dataDxfId="2"/>
+    <tableColumn id="1" name="x_barra" dataDxfId="1"/>
+    <tableColumn id="2" name="f(x_barra)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -441,8 +441,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>